<commit_message>
Update TCO Analysis Template with new calculations
</commit_message>
<xml_diff>
--- a/TCO_Analysis_Template.xlsx
+++ b/TCO_Analysis_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JerryCho0702\Desktop\Python\Total-Cost-of-Ownership\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAD66DC-F67D-4228-87FF-0DC5DE33E95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F2E516-BCB0-4158-B10E-7C3F124E2C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="10776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="10776" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input Parameters (輸入參數)" sheetId="1" r:id="rId1"/>
@@ -164,26 +164,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -488,16 +475,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="34.29296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1171875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.87890625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.29296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.87890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -512,68 +499,68 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>10000</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>2000</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>3000</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>1000</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="4" t="s">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>0.02</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -589,155 +576,156 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="A1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.234375" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.64453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1171875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1171875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5859375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.76171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.3515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.8203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.76171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.17578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.29296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.9375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" ht="30.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>10000</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>2000</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>3000</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>5000</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>15000</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>15000</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>0</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>2040</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>3060</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>5100</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>5100</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>20100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>0</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>2080.8000000000002</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>3121.2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>5202</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>5202</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>25302</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>0</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>2122.42</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>3183.62</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>5306.04</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>5306.04</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>30608.04</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>0</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>2164.86</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>3247.3</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>5412.16</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>5412.16</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>36020.199999999997</v>
       </c>
     </row>
@@ -751,15 +739,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="28" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.3515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -771,34 +759,34 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>26020.2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>35020.199999999997</v>
       </c>
     </row>

</xml_diff>